<commit_message>
correct some syntax errors mainly in the handle_excel section.py
</commit_message>
<xml_diff>
--- a/data/xinyangapitesting.xlsx
+++ b/data/xinyangapitesting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyang/Documents/Lemon Python Learning/API-Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CC5C4E-BDD9-4648-9B78-28A88ED6D6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FC5746-BDE7-6B43-8EB8-C12B36895915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30620" yWindow="1260" windowWidth="29660" windowHeight="15800" activeTab="1" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
+    <workbookView xWindow="-29100" yWindow="3760" windowWidth="29660" windowHeight="15800" activeTab="1" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>url</t>
   </si>
@@ -370,25 +370,31 @@
 ""select status from tz_order where order_number = '#orderNumbers#'"":1}"</t>
   </si>
   <si>
-    <t>https://openapiv5.ketangpai.com//UserApi/login</t>
-  </si>
-  <si>
     <t>{"Content-Type":"application/json"}</t>
   </si>
   <si>
-    <t>{"email":"2378807139@qq.com ","password":"123456",null,true}</t>
-  </si>
-  <si>
     <t>{"status":1,"code":10000,"message":"访问成功"}</t>
   </si>
   <si>
-    <t>https://openapiv6.ketangpai.com//UserApi/login</t>
-  </si>
-  <si>
     <t>{"email":"2378807139@qq.com ","password":"lemon"}</t>
   </si>
   <si>
     <t>{"status":0,"code":"30508","message":"登录失败"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">success_case </t>
+  </si>
+  <si>
+    <t>failed_case</t>
+  </si>
+  <si>
+    <t>request_parameter</t>
+  </si>
+  <si>
+    <t>https://openapiv5.ketangpai.com/UserApi/login</t>
+  </si>
+  <si>
+    <t>{"email":"2378807139@qq.com ","password":"123456"}</t>
   </si>
 </sst>
 </file>
@@ -465,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -480,6 +486,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1056,7 +1065,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1086,7 +1095,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1099,36 +1108,58 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="D2" s="3" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="D3" s="3" t="s">
-        <v>50</v>
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H3" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{5EA1B580-AFE8-8F48-8E2E-7EC31B3DB8BA}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{8AE3FE47-8D63-164B-A522-C4903D427DDB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding extraction, replacement method
</commit_message>
<xml_diff>
--- a/data/xinyangapitesting.xlsx
+++ b/data/xinyangapitesting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyang/Documents/Lemon Python Learning/API-Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FC5746-BDE7-6B43-8EB8-C12B36895915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5A5324-2ED6-5544-9A2C-CD74A0F1829E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29100" yWindow="3760" windowWidth="29660" windowHeight="15800" activeTab="1" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
+    <workbookView xWindow="-33400" yWindow="2840" windowWidth="32180" windowHeight="16680" activeTab="1" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
   <si>
     <t>url</t>
   </si>
@@ -373,35 +373,118 @@
     <t>{"Content-Type":"application/json"}</t>
   </si>
   <si>
-    <t>{"status":1,"code":10000,"message":"访问成功"}</t>
-  </si>
-  <si>
-    <t>{"email":"2378807139@qq.com ","password":"lemon"}</t>
-  </si>
-  <si>
-    <t>{"status":0,"code":"30508","message":"登录失败"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">success_case </t>
-  </si>
-  <si>
-    <t>failed_case</t>
-  </si>
-  <si>
     <t>request_parameter</t>
   </si>
   <si>
-    <t>https://openapiv5.ketangpai.com/UserApi/login</t>
-  </si>
-  <si>
-    <t>{"email":"2378807139@qq.com ","password":"123456"}</t>
+    <t>{"principal": "lemon_py", "credentials": "12345678", "appType": 3, "loginType": 0}</t>
+  </si>
+  <si>
+    <t>{"$..nickName":"lemon_py","$..enabled":true}</t>
+  </si>
+  <si>
+    <t>{"principal": "", "credentials": "lemon123456", "appType": 3, "loginType": 0}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>{"text":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>账号或密码不正确</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"}</t>
+    </r>
+  </si>
+  <si>
+    <t>{"principal": "lem", "credentials": "lemon123456", "appType": 3, "loginType": 0}</t>
+  </si>
+  <si>
+    <t>{"principal": "lemon_autoXXXXXXXXXXXXXXXXX", "credentials": "lemon123456", "appType": 3, "loginType": 0}</t>
+  </si>
+  <si>
+    <t>{"principal": "lemon!", "credentials": "lemon123456", "appType": 3, "loginType": 0}</t>
+  </si>
+  <si>
+    <t>{"principal": "lemon_autoxx", "credentials": "lemon123456", "appType": 3, "loginType": 0}</t>
+  </si>
+  <si>
+    <t>{"principal": "lemon_py", "credentials": "", "appType": 3, "loginType": 0}</t>
+  </si>
+  <si>
+    <t>{"principal": "lemon_py", "credentials": "lemon123", "appType": 3, "loginType": 0}</t>
+  </si>
+  <si>
+    <t>login_001</t>
+  </si>
+  <si>
+    <t>login_002</t>
+  </si>
+  <si>
+    <t>login_003</t>
+  </si>
+  <si>
+    <t>login_004</t>
+  </si>
+  <si>
+    <t>login_005</t>
+  </si>
+  <si>
+    <t>login_006</t>
+  </si>
+  <si>
+    <t>login_007</t>
+  </si>
+  <si>
+    <t>login_008</t>
+  </si>
+  <si>
+    <t>Login_in_sucessful</t>
+  </si>
+  <si>
+    <t>Login_in_fail</t>
+  </si>
+  <si>
+    <t>Login_in_fail (usename&lt;4letters)</t>
+  </si>
+  <si>
+    <t>Login_in_fail (usename&gt;16letters)</t>
+  </si>
+  <si>
+    <t>Login_in_fail (usename has special charaters)</t>
+  </si>
+  <si>
+    <t>Login_in_fail (not registered username)</t>
+  </si>
+  <si>
+    <t>Login_in_fail (no password)</t>
+  </si>
+  <si>
+    <t>Login_in_fail (password is wrong)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -443,6 +526,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -471,7 +573,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -487,8 +589,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -827,11 +932,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562F5F3D-E2EA-9240-9A70-317BC054BC3A}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="29.5" customWidth="1"/>
@@ -844,7 +949,7 @@
     <col min="9" max="9" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -873,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="51">
       <c r="A2">
         <v>1</v>
       </c>
@@ -899,7 +1004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="17">
       <c r="A3">
         <v>2</v>
       </c>
@@ -919,7 +1024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="17">
       <c r="A4">
         <v>3</v>
       </c>
@@ -939,7 +1044,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="66" customHeight="1">
       <c r="A5">
         <v>4</v>
       </c>
@@ -959,7 +1064,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="61" customHeight="1">
       <c r="A6">
         <v>5</v>
       </c>
@@ -982,7 +1087,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="48">
       <c r="A7">
         <v>6</v>
       </c>
@@ -999,7 +1104,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="48">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1019,7 +1124,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="136">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1062,15 +1167,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F1B2B2-99C6-F74C-BE60-04C41AAB74CA}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="35.83203125" customWidth="1"/>
     <col min="5" max="5" width="35.6640625" customWidth="1"/>
     <col min="6" max="6" width="28.6640625" customWidth="1"/>
@@ -1078,7 +1184,7 @@
     <col min="8" max="8" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1095,7 +1201,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1107,58 +1213,202 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:9" ht="51">
+      <c r="A2" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="51">
+      <c r="A3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="51">
+      <c r="A4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="62" customHeight="1">
+      <c r="A5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="51">
+      <c r="A6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F6" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="G6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="7" spans="1:9" ht="51">
+      <c r="A7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="3"/>
+      <c r="F7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="51">
+      <c r="A8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="51">
+      <c r="A9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{5EA1B580-AFE8-8F48-8E2E-7EC31B3DB8BA}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{8AE3FE47-8D63-164B-A522-C4903D427DDB}"/>
+    <hyperlink ref="D2" r:id="rId1" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{82A1EC3F-1BCD-BA4F-AB17-CB90C26045C6}"/>
+    <hyperlink ref="D3" r:id="rId2" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{9C777156-D4CD-D949-A755-212E193A73A8}"/>
+    <hyperlink ref="D7" r:id="rId3" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{0744FA7E-F2C1-7A45-8D4B-B8476BD80E72}"/>
+    <hyperlink ref="D8" r:id="rId4" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{AAF26CE1-F5FE-B843-B7F3-11A9CA25263C}"/>
+    <hyperlink ref="D9" r:id="rId5" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{94815DF5-EB56-8649-96D0-7C8242A4C742}"/>
+    <hyperlink ref="D4" r:id="rId6" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{B3252E53-9C29-F947-B9CF-A85D66A37AFB}"/>
+    <hyperlink ref="D5" r:id="rId7" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{9FE81995-C89B-2642-896B-5826C6C0774B}"/>
+    <hyperlink ref="D6" r:id="rId8" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{33EDB075-AB10-FF43-B810-8C0692E3CD88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
make some more updates on register cases
</commit_message>
<xml_diff>
--- a/data/xinyangapitesting.xlsx
+++ b/data/xinyangapitesting.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyang/Documents/Lemon Python Learning/API-Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5A5324-2ED6-5544-9A2C-CD74A0F1829E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FEC969-E3BA-5B42-8A2D-10C51B9405BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33400" yWindow="2840" windowWidth="32180" windowHeight="16680" activeTab="1" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="login" sheetId="2" r:id="rId2"/>
+    <sheet name="register " sheetId="3" r:id="rId1"/>
+    <sheet name="busniess flow" sheetId="1" r:id="rId2"/>
+    <sheet name="login" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="89">
   <si>
     <t>url</t>
   </si>
@@ -478,13 +479,59 @@
   </si>
   <si>
     <t>Login_in_fail (password is wrong)</t>
+  </si>
+  <si>
+    <t>Send registration SMS verification code</t>
+  </si>
+  <si>
+    <t>Send and verify registration SMS verification code</t>
+  </si>
+  <si>
+    <t>Registration API request</t>
+  </si>
+  <si>
+    <t>http://shop.lemonban.com:8107/user/sendRegisterSms</t>
+  </si>
+  <si>
+    <t>http://shop.lemonban.com:8107/user/checkRegisterSms</t>
+  </si>
+  <si>
+    <t>http://shop.lemonban.com:8107/user/registerOrBindUser</t>
+  </si>
+  <si>
+    <t>{ "Content-Type": "application/json; charset=UTF-8"}</t>
+  </si>
+  <si>
+    <t>{"Content-Type": "application/json; charset=UTF-8"}</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>{"mobile":"#gen_unregister_phone()#"}</t>
+  </si>
+  <si>
+    <t>{"mobile":"#gen_unregister_phone#","validCode":"#mobile_code#"}</t>
+  </si>
+  <si>
+    <t>{"appType":3,"checkRegisterSmsFlag":"#check_code#","mobile":"#gen_unregister_phone#","userName":"#gen_unregister_name()#","password":"123456","registerOrBind":1,"validateType":1}</t>
+  </si>
+  <si>
+    <t>{"check_code":"text"}</t>
+  </si>
+  <si>
+    <t>{"mobile_code":
+"select mobile_code  from tz_sms_log where user_phone='#gen_unregister_phone#' order by rec_date desc limit 1;"}</t>
+  </si>
+  <si>
+    <t>pre_sql</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -545,6 +592,12 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -573,7 +626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -593,6 +646,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -929,6 +985,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70910427-306D-C74C-9DEC-96EC5E562EFF}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="47.5" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" customWidth="1"/>
+    <col min="6" max="6" width="57.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" customWidth="1"/>
+    <col min="9" max="9" width="34.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="34">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="85">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{4CD51D07-038B-C44B-BBA9-2BFAA6F20ACD}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{E5CD9B57-0467-334C-965B-FD7D6EA178F4}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{87B21301-FBAB-9F42-A44B-049931E53256}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562F5F3D-E2EA-9240-9A70-317BC054BC3A}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -1165,12 +1350,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F1B2B2-99C6-F74C-BE60-04C41AAB74CA}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
add the put request code to request api file
</commit_message>
<xml_diff>
--- a/data/xinyangapitesting.xlsx
+++ b/data/xinyangapitesting.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyang/Documents/Lemon Python Learning/API-Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FEC969-E3BA-5B42-8A2D-10C51B9405BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B0F379-C47D-C74F-A384-89BFB378E32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="16020" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
   </bookViews>
   <sheets>
-    <sheet name="register " sheetId="3" r:id="rId1"/>
-    <sheet name="busniess flow" sheetId="1" r:id="rId2"/>
-    <sheet name="login" sheetId="2" r:id="rId3"/>
+    <sheet name="test_register" sheetId="3" r:id="rId1"/>
+    <sheet name="login" sheetId="2" r:id="rId2"/>
+    <sheet name="busniess flow" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -484,9 +484,6 @@
     <t>Send registration SMS verification code</t>
   </si>
   <si>
-    <t>Send and verify registration SMS verification code</t>
-  </si>
-  <si>
     <t>Registration API request</t>
   </si>
   <si>
@@ -525,6 +522,9 @@
   </si>
   <si>
     <t>pre_sql</t>
+  </si>
+  <si>
+    <t>press next step to verify registration SMS verification code</t>
   </si>
 </sst>
 </file>
@@ -988,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70910427-306D-C74C-9DEC-96EC5E562EFF}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1031,7 +1031,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1</v>
@@ -1045,16 +1045,16 @@
         <v>74</v>
       </c>
       <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
         <v>82</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="34">
@@ -1062,19 +1062,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="85">
@@ -1082,25 +1082,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
         <v>79</v>
       </c>
-      <c r="E4" t="s">
-        <v>80</v>
-      </c>
       <c r="F4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1114,6 +1114,255 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F1B2B2-99C6-F74C-BE60-04C41AAB74CA}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="35.83203125" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="34.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="51">
+      <c r="A2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="51">
+      <c r="A3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="51">
+      <c r="A4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="62" customHeight="1">
+      <c r="A5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="51">
+      <c r="A6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="51">
+      <c r="A7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="51">
+      <c r="A8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="51">
+      <c r="A9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{82A1EC3F-1BCD-BA4F-AB17-CB90C26045C6}"/>
+    <hyperlink ref="D3" r:id="rId2" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{9C777156-D4CD-D949-A755-212E193A73A8}"/>
+    <hyperlink ref="D7" r:id="rId3" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{0744FA7E-F2C1-7A45-8D4B-B8476BD80E72}"/>
+    <hyperlink ref="D8" r:id="rId4" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{AAF26CE1-F5FE-B843-B7F3-11A9CA25263C}"/>
+    <hyperlink ref="D9" r:id="rId5" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{94815DF5-EB56-8649-96D0-7C8242A4C742}"/>
+    <hyperlink ref="D4" r:id="rId6" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{B3252E53-9C29-F947-B9CF-A85D66A37AFB}"/>
+    <hyperlink ref="D5" r:id="rId7" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{9FE81995-C89B-2642-896B-5826C6C0774B}"/>
+    <hyperlink ref="D6" r:id="rId8" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{33EDB075-AB10-FF43-B810-8C0692E3CD88}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562F5F3D-E2EA-9240-9A70-317BC054BC3A}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -1348,253 +1597,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F1B2B2-99C6-F74C-BE60-04C41AAB74CA}">
-  <dimension ref="A1:I9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="35.83203125" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" customWidth="1"/>
-    <col min="8" max="8" width="34.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="51">
-      <c r="A2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="51">
-      <c r="A3" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="51">
-      <c r="A4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="62" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="51">
-      <c r="A6" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="51">
-      <c r="A7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="51">
-      <c r="A8" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="51">
-      <c r="A9" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{82A1EC3F-1BCD-BA4F-AB17-CB90C26045C6}"/>
-    <hyperlink ref="D3" r:id="rId2" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{9C777156-D4CD-D949-A755-212E193A73A8}"/>
-    <hyperlink ref="D7" r:id="rId3" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{0744FA7E-F2C1-7A45-8D4B-B8476BD80E72}"/>
-    <hyperlink ref="D8" r:id="rId4" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{AAF26CE1-F5FE-B843-B7F3-11A9CA25263C}"/>
-    <hyperlink ref="D9" r:id="rId5" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{94815DF5-EB56-8649-96D0-7C8242A4C742}"/>
-    <hyperlink ref="D4" r:id="rId6" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{B3252E53-9C29-F947-B9CF-A85D66A37AFB}"/>
-    <hyperlink ref="D5" r:id="rId7" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{9FE81995-C89B-2642-896B-5826C6C0774B}"/>
-    <hyperlink ref="D6" r:id="rId8" tooltip="http://shop.lemonban.com:8107/login" xr:uid="{33EDB075-AB10-FF43-B810-8C0692E3CD88}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added another test case
</commit_message>
<xml_diff>
--- a/data/xinyangapitesting.xlsx
+++ b/data/xinyangapitesting.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyang/Documents/Lemon Python Learning/API-Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E165D1-8CC0-C94C-BCF4-7BF06D7A5F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4575163F-6902-A148-922D-DEF11AE19BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33240" yWindow="5320" windowWidth="37280" windowHeight="16020" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
+    <workbookView xWindow="5560" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="2" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
   </bookViews>
   <sheets>
     <sheet name="test_register" sheetId="3" r:id="rId1"/>
     <sheet name="login" sheetId="2" r:id="rId2"/>
-    <sheet name="busniess flow" sheetId="1" r:id="rId3"/>
+    <sheet name="test_busniess_flow" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -988,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70910427-306D-C74C-9DEC-96EC5E562EFF}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1366,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562F5F3D-E2EA-9240-9A70-317BC054BC3A}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
some more modifications 22/09
</commit_message>
<xml_diff>
--- a/data/xinyangapitesting.xlsx
+++ b/data/xinyangapitesting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyang/Documents/Lemon Python Learning/API-Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961B6E95-2A6B-5E40-8A38-8AE45709A1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C635F13A-6297-C241-8AF3-6A7341666D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="500" windowWidth="26120" windowHeight="15380" activeTab="2" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
+    <workbookView xWindow="540" yWindow="500" windowWidth="27940" windowHeight="15380" activeTab="2" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
   </bookViews>
   <sheets>
     <sheet name="test_register" sheetId="3" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>get</t>
   </si>
   <si>
-    <t>shop.lemonban.com:8107/search/searchProdPage</t>
-  </si>
-  <si>
     <t>{"prodName":"真皮圆筒包"}</t>
   </si>
   <si>
@@ -519,6 +516,9 @@
   </si>
   <si>
     <t>{"access_token":"$..access_token","token_type":"$..token_type"}</t>
+  </si>
+  <si>
+    <t>http://shop.lemonban.com:8107/search/searchProdPage</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1016,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1025,7 +1025,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1</v>
@@ -1036,19 +1036,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
         <v>78</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="85">
@@ -1056,25 +1056,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="51">
@@ -1082,19 +1082,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
         <v>75</v>
       </c>
-      <c r="E4" t="s">
-        <v>76</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1143,7 +1143,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1157,10 +1157,10 @@
     </row>
     <row r="2" spans="1:9" ht="51">
       <c r="A2" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>9</v>
@@ -1169,22 +1169,22 @@
         <v>10</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="51">
       <c r="A3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>9</v>
@@ -1193,22 +1193,22 @@
         <v>10</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="51">
       <c r="A4" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>9</v>
@@ -1217,21 +1217,21 @@
         <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="62" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
@@ -1240,21 +1240,21 @@
         <v>10</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="51">
       <c r="A6" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>9</v>
@@ -1263,21 +1263,21 @@
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="51">
       <c r="A7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>9</v>
@@ -1286,21 +1286,21 @@
         <v>10</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="51">
       <c r="A8" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>9</v>
@@ -1309,21 +1309,21 @@
         <v>10</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="51">
       <c r="A9" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>9</v>
@@ -1332,13 +1332,13 @@
         <v>10</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1360,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562F5F3D-E2EA-9240-9A70-317BC054BC3A}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1394,7 +1394,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1406,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="34">
@@ -1423,7 +1423,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>11</v>
@@ -1432,7 +1432,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="17">
@@ -1445,14 +1445,14 @@
       <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="H3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="17">
@@ -1460,19 +1460,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="66" customHeight="1">
@@ -1480,19 +1480,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="61" customHeight="1">
@@ -1500,22 +1500,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
       <c r="H6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="48">
@@ -1523,16 +1523,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="48">
@@ -1540,19 +1540,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="136">
@@ -1560,28 +1560,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" t="s">
         <v>39</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>40</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1590,6 +1590,7 @@
     <hyperlink ref="D4" r:id="rId2" xr:uid="{EA0507DB-F307-EB40-A539-C0D8885C4B36}"/>
     <hyperlink ref="D6" r:id="rId3" xr:uid="{C52EC358-BD85-4A44-8128-30A17D00202F}"/>
     <hyperlink ref="D9" r:id="rId4" xr:uid="{E707AACC-01C5-CA4F-A462-67DAB27B3CA3}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{A53AEE31-FA46-4A4F-ACE4-E20E86943EFA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
added allure, made some update on the extraction files
</commit_message>
<xml_diff>
--- a/data/xinyangapitesting.xlsx
+++ b/data/xinyangapitesting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyang/Documents/Lemon Python Learning/API-Automation/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyangzhang/Documents/Pycharm/API-Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C635F13A-6297-C241-8AF3-6A7341666D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC1C956-F8C4-5244-939D-11ACEE207DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="500" windowWidth="27940" windowHeight="15380" activeTab="2" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
+    <workbookView xWindow="1840" yWindow="7000" windowWidth="42040" windowHeight="18800" activeTab="2" xr2:uid="{2C3AEDAD-F0D7-0E4E-8199-4917A5FF045F}"/>
   </bookViews>
   <sheets>
     <sheet name="test_register" sheetId="3" r:id="rId1"/>
@@ -240,106 +240,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>{"prodId"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>:#prodId</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">{"basketId": 0, "count": 1, "prodId": </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>#prodId#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, "shopId": 1, "skuId": </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>#skuId#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>{"addrId": 0, "basketIds": [</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>#basketId#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>], "couponIds": [], "isScorePay": 0, "userChangeCoupon": 0,       "userUseScore": 0}</t>
-    </r>
-  </si>
-  <si>
     <t>submit the order</t>
   </si>
   <si>
@@ -519,6 +419,106 @@
   </si>
   <si>
     <t>http://shop.lemonban.com:8107/search/searchProdPage</t>
+  </si>
+  <si>
+    <r>
+      <t>{"prodId"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>:"#prodId</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>#"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{"basketId": 0, "count": 1, "prodId": "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>#prodId#"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, "shopId": 1, "skuId": "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>#skuId#"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{"addrId": 0, "basketIds": "[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>#basketId#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>]", "couponIds": [], "isScorePay": 0, "userChangeCoupon": 0,       "userUseScore": 0}</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1016,7 +1016,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1025,7 +1025,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1</v>
@@ -1036,19 +1036,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
         <v>72</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>75</v>
-      </c>
-      <c r="F2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="85">
@@ -1056,25 +1056,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" t="s">
         <v>76</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="51">
@@ -1082,19 +1082,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1143,7 +1143,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1157,10 +1157,10 @@
     </row>
     <row r="2" spans="1:9" ht="51">
       <c r="A2" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>9</v>
@@ -1169,22 +1169,22 @@
         <v>10</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="51">
       <c r="A3" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>9</v>
@@ -1193,22 +1193,22 @@
         <v>10</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="51">
       <c r="A4" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>9</v>
@@ -1217,21 +1217,21 @@
         <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="62" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
@@ -1240,21 +1240,21 @@
         <v>10</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="51">
       <c r="A6" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>9</v>
@@ -1263,21 +1263,21 @@
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="51">
       <c r="A7" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>9</v>
@@ -1286,21 +1286,21 @@
         <v>10</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="51">
       <c r="A8" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>9</v>
@@ -1309,21 +1309,21 @@
         <v>10</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="51">
       <c r="A9" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>9</v>
@@ -1332,13 +1332,13 @@
         <v>10</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1361,7 +1361,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1394,7 +1394,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1406,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="34">
@@ -1423,7 +1423,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>11</v>
@@ -1432,7 +1432,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="17">
@@ -1446,7 +1446,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>15</v>
@@ -1469,7 +1469,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>24</v>
@@ -1492,7 +1492,7 @@
         <v>32</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="61" customHeight="1">
@@ -1518,7 +1518,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="48">
+    <row r="7" spans="1:10" ht="32">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="48">
+    <row r="8" spans="1:10" ht="32">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>32</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="136">
@@ -1560,28 +1560,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="G9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>